<commit_message>
maj sosu repertoire total files
</commit_message>
<xml_diff>
--- a/modele.xlsx
+++ b/modele.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eric\python\perso\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87EBED75-7040-4BE9-9D41-DF10F8F5985F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C6087F-E687-45DE-8E3F-D2A5535D8CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="1440" windowWidth="10965" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>dossier</t>
   </si>
   <si>
-    <t>nb_all</t>
-  </si>
-  <si>
-    <t>nb_dos</t>
-  </si>
-  <si>
-    <t>nb_file</t>
+    <t>Nombre de fichiers dans le dossier</t>
   </si>
 </sst>
 </file>
@@ -386,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -395,20 +389,15 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
simplification uniquement les fichiers des sub
</commit_message>
<xml_diff>
--- a/modele.xlsx
+++ b/modele.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eric\python\perso\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C6087F-E687-45DE-8E3F-D2A5535D8CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECD740E-0AA6-4D1D-9690-B434FAA9F03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="1440" windowWidth="10965" windowHeight="9990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -95,11 +95,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,20 +387,20 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61.42578125" customWidth="1"/>
-    <col min="2" max="2" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
copy et toal size
</commit_message>
<xml_diff>
--- a/modele.xlsx
+++ b/modele.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eric\python\perso\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECD740E-0AA6-4D1D-9690-B434FAA9F03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AAD2E26-E5EB-407E-A069-8F1A0DD8F73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="750" windowWidth="11400" windowHeight="7695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="dossier">DATA!$A$1:$B$7</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -387,7 +390,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>